<commit_message>
Update Navbar And Bug Dashboard Admin Chart Data
</commit_message>
<xml_diff>
--- a/porto-import.xlsx
+++ b/porto-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dana\Repo\my-project\laravel\laravel-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89224FDC-B94C-EB45-8501-23E70A00D161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCF1B9F-1C9E-4F59-9B5E-274BE50762E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{AED53BD5-FCBC-0B4D-90FE-219E4D0BFD22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AED53BD5-FCBC-0B4D-90FE-219E4D0BFD22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,15 +41,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>judul 1</t>
-  </si>
-  <si>
-    <t>link 1</t>
-  </si>
-  <si>
-    <t>deskripsi singkat 1</t>
-  </si>
-  <si>
     <t>deskripsi_singkat</t>
   </si>
   <si>
@@ -65,16 +56,25 @@
     <t>id</t>
   </si>
   <si>
-    <t>Judul 2</t>
-  </si>
-  <si>
     <t>asd</t>
   </si>
   <si>
-    <t>link 2</t>
-  </si>
-  <si>
-    <t>deskripsi singkat 2</t>
+    <t>judul 3</t>
+  </si>
+  <si>
+    <t>Judul 4</t>
+  </si>
+  <si>
+    <t>deskripsi singkat 3</t>
+  </si>
+  <si>
+    <t>deskripsi singkat 4</t>
+  </si>
+  <si>
+    <t>link 3</t>
+  </si>
+  <si>
+    <t>link 4</t>
   </si>
 </sst>
 </file>
@@ -429,60 +429,60 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>